<commit_message>
BOM, BOM Template, Rowan Rocketry Logo
- Finished pyro controller BOM
- Created template for BOMs
- Created a footprint for adding the Rowan Rocketry logo to PCBs
</commit_message>
<xml_diff>
--- a/Pyro-Controller/bom/Pyro-Controller.xlsx
+++ b/Pyro-Controller/bom/Pyro-Controller.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Reference</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Screw_Terminal_01x02</t>
   </si>
   <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/640/1751248.pdf</t>
+    <t>q</t>
   </si>
   <si>
     <t>TerminalBlock_Phoenix:TerminalBlock_Phoenix_PT-1,5-2-3.5-H_1x02_P3.50mm_Horizontal</t>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">Phoenix Contact</t>
   </si>
   <si>
-    <t>Digikey</t>
+    <t>https://www.digikey.com/en/products/detail/phoenix-contact/1751248/2511016</t>
   </si>
   <si>
     <t>J2</t>
@@ -72,6 +72,9 @@
     <t xml:space="preserve">Sullins Connector Solutions</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/NPPN031BFCN-RC/804805</t>
+  </si>
+  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
     <t xml:space="preserve">Vishay Siliconix</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-siliconix/SIS454DN-T1-GE3/2441826?s=N4IgTCBcDaIMoEs4BYCsyAiA5EBdAvkA</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -99,15 +105,27 @@
     <t>YAGEO</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-073K3L/726757?_gl=1*oprbzy*_up*MQ..&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2qquIi0HITcnSJzEILMOtvyCB9wPLUQOH5qAcVxd7LGVxbBaQts_tIaAkVREALw_wcB</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-071KL/726677?_gl=1*1an2o6r*_up*MQ..&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2qquIi0HITcnSJzEILMOtvyCB9wPLUQOH5qAcVxd7LGVxbBaQts_tIaAkVREALw_wcB</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-13100KL/13694230?_gl=1*1eq4xmo*_up*MQ..&amp;gclid=Cj0KCQjwj4K5BhDYARIsAD1Ly2qquIi0HITcnSJzEILMOtvyCB9wPLUQOH5qAcVxd7LGVxbBaQts_tIaAkVREALw_wcB</t>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC0603JR-0727KL/726752</t>
+  </si>
+  <si>
     <t>TP1,TP2,TP3</t>
   </si>
   <si>
@@ -121,6 +139,9 @@
   </si>
   <si>
     <t xml:space="preserve">Keystone Electronics</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/5000/255326</t>
   </si>
 </sst>
 </file>
@@ -649,7 +670,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="11.36328125"/>
     <col bestFit="1" min="2" max="2" width="20.453125"/>
@@ -724,152 +745,152 @@
         <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2">
         <v>3.2999999999999998</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4">
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5">
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E9">
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2" tooltip=""/>
-    <hyperlink r:id="rId2" ref="G3" tooltip=""/>
+    <hyperlink r:id="rId2" ref="G3"/>
     <hyperlink r:id="rId3" ref="G4" tooltip=""/>
     <hyperlink r:id="rId4" ref="G5" tooltip=""/>
     <hyperlink r:id="rId5" ref="G6" tooltip=""/>

</xml_diff>